<commit_message>
finalize and test driver
</commit_message>
<xml_diff>
--- a/misc/config.xlsx
+++ b/misc/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tp\Documents\GITHUB STUFF\ranklogit\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8AB292-7140-450F-97D4-15C8DE423594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D51233-A405-4698-839C-972E34AAD8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">Priors:	</t>
   </si>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +176,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,16 +226,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,7 +520,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +538,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -535,7 +546,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B3" t="s">
@@ -543,7 +554,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
@@ -551,7 +562,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
@@ -559,7 +570,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
@@ -567,7 +578,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
@@ -575,7 +586,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
@@ -583,7 +594,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
@@ -591,7 +602,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
@@ -599,7 +610,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
@@ -607,7 +618,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B12" t="s">
@@ -615,7 +626,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
@@ -623,7 +634,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B14" t="s">
@@ -631,7 +642,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B15" t="s">
@@ -648,7 +659,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,22 +667,25 @@
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -688,7 +702,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3">
@@ -705,7 +719,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -722,7 +736,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -739,7 +753,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6">
@@ -756,7 +770,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7">
@@ -773,7 +787,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8">
@@ -790,7 +804,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B9">
@@ -807,7 +821,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10">
@@ -824,7 +838,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11">
@@ -841,7 +855,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12">
@@ -858,7 +872,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13">
@@ -875,7 +889,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14">
@@ -892,7 +906,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15">

</xml_diff>